<commit_message>
Ermögliche Umläufe und Pausen
</commit_message>
<xml_diff>
--- a/Outputdateien/Test1.xlsx
+++ b/Outputdateien/Test1.xlsx
@@ -894,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>2E-06</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <v>20</v>
@@ -938,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>5E-06</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>20</v>
@@ -982,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>1E-05</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>20</v>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <v>1.6E-05</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>20</v>
@@ -1070,7 +1070,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>2.2E-05</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
         <v>20</v>
@@ -1114,7 +1114,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>2.9E-05</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2">
         <v>20</v>
@@ -1158,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>3.6E-05</v>
+        <v>36.00000000000001</v>
       </c>
       <c r="D9" s="2">
         <v>20</v>
@@ -1202,7 +1202,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>4.5E-05</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2">
         <v>20</v>
@@ -1246,7 +1246,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <v>5.3E-05</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2">
         <v>20</v>
@@ -1290,7 +1290,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>6.2E-05</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2">
         <v>20</v>
@@ -1334,7 +1334,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>7.3E-05</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2">
         <v>20</v>
@@ -1378,7 +1378,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2">
-        <v>8.3E-05</v>
+        <v>83</v>
       </c>
       <c r="D14" s="2">
         <v>20</v>
@@ -1422,7 +1422,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2">
-        <v>9.399999999999999E-05</v>
+        <v>94</v>
       </c>
       <c r="D15" s="2">
         <v>20</v>
@@ -1466,7 +1466,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="2">
-        <v>0.000104</v>
+        <v>104</v>
       </c>
       <c r="D16" s="2">
         <v>20</v>
@@ -1510,7 +1510,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="2">
-        <v>0.000114</v>
+        <v>114</v>
       </c>
       <c r="D17" s="2">
         <v>20</v>
@@ -1554,7 +1554,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
-        <v>0.000123</v>
+        <v>123</v>
       </c>
       <c r="D18" s="2">
         <v>20</v>
@@ -1598,7 +1598,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="2">
-        <v>0.000133</v>
+        <v>133</v>
       </c>
       <c r="D19" s="2">
         <v>20</v>
@@ -1642,7 +1642,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2">
-        <v>0.000142</v>
+        <v>142</v>
       </c>
       <c r="D20" s="2">
         <v>20</v>
@@ -1686,7 +1686,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="2">
-        <v>0.000152</v>
+        <v>152</v>
       </c>
       <c r="D21" s="2">
         <v>20</v>
@@ -1730,7 +1730,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="2">
-        <v>0.000162</v>
+        <v>162</v>
       </c>
       <c r="D22" s="2">
         <v>20</v>
@@ -1774,7 +1774,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2">
-        <v>0.000172</v>
+        <v>172</v>
       </c>
       <c r="D23" s="2">
         <v>20</v>
@@ -1818,7 +1818,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="2">
-        <v>0.000182</v>
+        <v>182</v>
       </c>
       <c r="D24" s="2">
         <v>20</v>
@@ -1862,7 +1862,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="2">
-        <v>0.000192</v>
+        <v>192</v>
       </c>
       <c r="D25" s="2">
         <v>20</v>
@@ -1906,7 +1906,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="2">
-        <v>0.000203</v>
+        <v>203</v>
       </c>
       <c r="D26" s="2">
         <v>20</v>
@@ -1950,7 +1950,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="2">
-        <v>0.000213</v>
+        <v>213</v>
       </c>
       <c r="D27" s="2">
         <v>20</v>
@@ -1994,7 +1994,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="2">
-        <v>0.000224</v>
+        <v>224</v>
       </c>
       <c r="D28" s="2">
         <v>20</v>
@@ -2038,7 +2038,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="2">
-        <v>0.000235</v>
+        <v>235</v>
       </c>
       <c r="D29" s="2">
         <v>20</v>
@@ -2082,7 +2082,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="2">
-        <v>0.000246</v>
+        <v>246</v>
       </c>
       <c r="D30" s="2">
         <v>20</v>
@@ -2126,7 +2126,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2">
-        <v>0.000258</v>
+        <v>258</v>
       </c>
       <c r="D31" s="2">
         <v>20</v>
@@ -2170,7 +2170,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="2">
-        <v>0.00027</v>
+        <v>270</v>
       </c>
       <c r="D32" s="2">
         <v>20</v>
@@ -2214,7 +2214,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="2">
-        <v>0.0002810000000000001</v>
+        <v>281</v>
       </c>
       <c r="D33" s="2">
         <v>20</v>
@@ -2258,7 +2258,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="2">
-        <v>0.000293</v>
+        <v>293</v>
       </c>
       <c r="D34" s="2">
         <v>20</v>
@@ -2302,7 +2302,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="2">
-        <v>0.000305</v>
+        <v>305</v>
       </c>
       <c r="D35" s="2">
         <v>20</v>
@@ -2346,7 +2346,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="2">
-        <v>0.000318</v>
+        <v>318</v>
       </c>
       <c r="D36" s="2">
         <v>20</v>
@@ -2390,7 +2390,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="2">
-        <v>0.000331</v>
+        <v>331</v>
       </c>
       <c r="D37" s="2">
         <v>20</v>
@@ -2434,7 +2434,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="2">
-        <v>0.000344</v>
+        <v>344</v>
       </c>
       <c r="D38" s="2">
         <v>20</v>
@@ -2478,7 +2478,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="2">
-        <v>0.0003570000000000001</v>
+        <v>357.0000000000001</v>
       </c>
       <c r="D39" s="2">
         <v>20</v>
@@ -2522,7 +2522,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="2">
-        <v>0.000371</v>
+        <v>371</v>
       </c>
       <c r="D40" s="2">
         <v>20</v>
@@ -2566,7 +2566,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="2">
-        <v>0.000384</v>
+        <v>384</v>
       </c>
       <c r="D41" s="2">
         <v>20</v>
@@ -2610,7 +2610,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="2">
-        <v>0.000397</v>
+        <v>397</v>
       </c>
       <c r="D42" s="2">
         <v>20</v>
@@ -2654,7 +2654,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="2">
-        <v>0.00041</v>
+        <v>410</v>
       </c>
       <c r="D43" s="2">
         <v>20</v>
@@ -2698,7 +2698,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="2">
-        <v>0.0004220000000000001</v>
+        <v>422.0000000000001</v>
       </c>
       <c r="D44" s="2">
         <v>20</v>
@@ -2742,7 +2742,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="2">
-        <v>0.000435</v>
+        <v>435</v>
       </c>
       <c r="D45" s="2">
         <v>20</v>
@@ -2786,7 +2786,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="2">
-        <v>0.000447</v>
+        <v>447</v>
       </c>
       <c r="D46" s="2">
         <v>20</v>
@@ -2830,7 +2830,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="2">
-        <v>0.000459</v>
+        <v>458.9999999999999</v>
       </c>
       <c r="D47" s="2">
         <v>20</v>
@@ -2874,7 +2874,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="2">
-        <v>0.000471</v>
+        <v>471.0000000000001</v>
       </c>
       <c r="D48" s="2">
         <v>20</v>
@@ -2918,7 +2918,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="2">
-        <v>0.000483</v>
+        <v>483</v>
       </c>
       <c r="D49" s="2">
         <v>20</v>
@@ -2962,7 +2962,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="2">
-        <v>0.000495</v>
+        <v>495</v>
       </c>
       <c r="D50" s="2">
         <v>20</v>
@@ -3006,7 +3006,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="2">
-        <v>0.000506</v>
+        <v>506</v>
       </c>
       <c r="D51" s="2">
         <v>20</v>
@@ -3050,7 +3050,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="2">
-        <v>0.000517</v>
+        <v>517</v>
       </c>
       <c r="D52" s="2">
         <v>20</v>
@@ -3094,7 +3094,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="2">
-        <v>0.000527</v>
+        <v>527</v>
       </c>
       <c r="D53" s="2">
         <v>20</v>
@@ -3138,7 +3138,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="2">
-        <v>0.000537</v>
+        <v>537</v>
       </c>
       <c r="D54" s="2">
         <v>20</v>
@@ -3182,7 +3182,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="2">
-        <v>0.0005470000000000001</v>
+        <v>547</v>
       </c>
       <c r="D55" s="2">
         <v>20</v>
@@ -3226,7 +3226,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="2">
-        <v>0.0005570000000000001</v>
+        <v>557</v>
       </c>
       <c r="D56" s="2">
         <v>20</v>
@@ -3270,7 +3270,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="2">
-        <v>0.000565</v>
+        <v>565</v>
       </c>
       <c r="D57" s="2">
         <v>20</v>
@@ -3314,7 +3314,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="2">
-        <v>0.000574</v>
+        <v>574</v>
       </c>
       <c r="D58" s="2">
         <v>20</v>
@@ -3358,7 +3358,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="2">
-        <v>0.000583</v>
+        <v>583</v>
       </c>
       <c r="D59" s="2">
         <v>20</v>
@@ -3402,7 +3402,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="2">
-        <v>0.0005920000000000001</v>
+        <v>592.0000000000001</v>
       </c>
       <c r="D60" s="2">
         <v>20</v>
@@ -3446,7 +3446,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="2">
-        <v>0.0005999999999999999</v>
+        <v>600</v>
       </c>
       <c r="D61" s="2">
         <v>20</v>
@@ -3490,7 +3490,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="2">
-        <v>0.0006089999999999999</v>
+        <v>609</v>
       </c>
       <c r="D62" s="2">
         <v>20</v>
@@ -3534,7 +3534,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="2">
-        <v>0.000616</v>
+        <v>616</v>
       </c>
       <c r="D63" s="2">
         <v>20</v>
@@ -3578,7 +3578,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="2">
-        <v>0.000623</v>
+        <v>623</v>
       </c>
       <c r="D64" s="2">
         <v>20</v>
@@ -3622,7 +3622,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="2">
-        <v>0.0006310000000000001</v>
+        <v>631</v>
       </c>
       <c r="D65" s="2">
         <v>20</v>
@@ -3666,7 +3666,7 @@
         <v>64</v>
       </c>
       <c r="C66" s="2">
-        <v>0.000639</v>
+        <v>639</v>
       </c>
       <c r="D66" s="2">
         <v>20</v>
@@ -3710,7 +3710,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="2">
-        <v>0.000648</v>
+        <v>648</v>
       </c>
       <c r="D67" s="2">
         <v>20</v>
@@ -3754,7 +3754,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="2">
-        <v>0.0006559999999999999</v>
+        <v>655.9999999999999</v>
       </c>
       <c r="D68" s="2">
         <v>20</v>
@@ -3798,7 +3798,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="2">
-        <v>0.000665</v>
+        <v>665</v>
       </c>
       <c r="D69" s="2">
         <v>20</v>
@@ -3842,7 +3842,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="2">
-        <v>0.0006729999999999999</v>
+        <v>672.9999999999999</v>
       </c>
       <c r="D70" s="2">
         <v>20</v>
@@ -3886,7 +3886,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="2">
-        <v>0.000681</v>
+        <v>680.9999999999999</v>
       </c>
       <c r="D71" s="2">
         <v>20</v>
@@ -3930,7 +3930,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="2">
-        <v>0.000687</v>
+        <v>687</v>
       </c>
       <c r="D72" s="2">
         <v>20</v>
@@ -3974,7 +3974,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="2">
-        <v>0.000692</v>
+        <v>692.0000000000001</v>
       </c>
       <c r="D73" s="2">
         <v>20</v>
@@ -4018,7 +4018,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="2">
-        <v>0.000696</v>
+        <v>696</v>
       </c>
       <c r="D74" s="2">
         <v>20</v>
@@ -4062,7 +4062,7 @@
         <v>73</v>
       </c>
       <c r="C75" s="2">
-        <v>0.0006990000000000001</v>
+        <v>699.0000000000001</v>
       </c>
       <c r="D75" s="2">
         <v>20</v>
@@ -4106,7 +4106,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="2">
-        <v>0.000702</v>
+        <v>702.0000000000001</v>
       </c>
       <c r="D76" s="2">
         <v>20</v>
@@ -4150,7 +4150,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="2">
-        <v>0.0007059999999999999</v>
+        <v>706</v>
       </c>
       <c r="D77" s="2">
         <v>20</v>
@@ -4194,7 +4194,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="2">
-        <v>0.0007099999999999999</v>
+        <v>710</v>
       </c>
       <c r="D78" s="2">
         <v>20</v>
@@ -4238,7 +4238,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="2">
-        <v>0.0007149999999999999</v>
+        <v>715</v>
       </c>
       <c r="D79" s="2">
         <v>20</v>
@@ -4282,7 +4282,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="2">
-        <v>0.0007190000000000001</v>
+        <v>719.0000000000001</v>
       </c>
       <c r="D80" s="2">
         <v>20</v>
@@ -4326,7 +4326,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="2">
-        <v>0.000725</v>
+        <v>725</v>
       </c>
       <c r="D81" s="2">
         <v>20</v>
@@ -4370,7 +4370,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="2">
-        <v>0.00073</v>
+        <v>730</v>
       </c>
       <c r="D82" s="2">
         <v>20</v>
@@ -4414,7 +4414,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="2">
-        <v>0.000736</v>
+        <v>736</v>
       </c>
       <c r="D83" s="2">
         <v>20</v>
@@ -4458,7 +4458,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="2">
-        <v>0.000741</v>
+        <v>741</v>
       </c>
       <c r="D84" s="2">
         <v>20</v>
@@ -4502,7 +4502,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="2">
-        <v>0.000746</v>
+        <v>746</v>
       </c>
       <c r="D85" s="2">
         <v>20</v>
@@ -4546,7 +4546,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="2">
-        <v>0.000752</v>
+        <v>752</v>
       </c>
       <c r="D86" s="2">
         <v>20</v>
@@ -4590,7 +4590,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="2">
-        <v>0.000757</v>
+        <v>757</v>
       </c>
       <c r="D87" s="2">
         <v>20</v>
@@ -4634,7 +4634,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="2">
-        <v>0.000763</v>
+        <v>763</v>
       </c>
       <c r="D88" s="2">
         <v>20</v>
@@ -4678,7 +4678,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="2">
-        <v>0.000768</v>
+        <v>768</v>
       </c>
       <c r="D89" s="2">
         <v>20</v>
@@ -4722,7 +4722,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="2">
-        <v>0.000773</v>
+        <v>773</v>
       </c>
       <c r="D90" s="2">
         <v>20</v>
@@ -4766,7 +4766,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="2">
-        <v>0.000778</v>
+        <v>778</v>
       </c>
       <c r="D91" s="2">
         <v>20</v>
@@ -4810,7 +4810,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="2">
-        <v>0.000782</v>
+        <v>782</v>
       </c>
       <c r="D92" s="2">
         <v>20</v>
@@ -4854,7 +4854,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="2">
-        <v>0.000785</v>
+        <v>785</v>
       </c>
       <c r="D93" s="2">
         <v>20</v>
@@ -4898,7 +4898,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2">
-        <v>0.000788</v>
+        <v>787.9999999999999</v>
       </c>
       <c r="D94" s="2">
         <v>20</v>
@@ -4942,7 +4942,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="2">
-        <v>0.0007920000000000001</v>
+        <v>792</v>
       </c>
       <c r="D95" s="2">
         <v>20</v>
@@ -4986,7 +4986,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="2">
-        <v>0.0007959999999999999</v>
+        <v>795.9999999999999</v>
       </c>
       <c r="D96" s="2">
         <v>20</v>
@@ -5030,7 +5030,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="2">
-        <v>0.0008</v>
+        <v>800</v>
       </c>
       <c r="D97" s="2">
         <v>20</v>
@@ -5074,7 +5074,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="2">
-        <v>0.0008029999999999999</v>
+        <v>802.9999999999999</v>
       </c>
       <c r="D98" s="2">
         <v>20</v>
@@ -5118,7 +5118,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="2">
-        <v>0.000809</v>
+        <v>809</v>
       </c>
       <c r="D99" s="2">
         <v>20</v>
@@ -5162,7 +5162,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="2">
-        <v>0.000812</v>
+        <v>812</v>
       </c>
       <c r="D100" s="2">
         <v>20</v>
@@ -5206,7 +5206,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="2">
-        <v>0.000816</v>
+        <v>816</v>
       </c>
       <c r="D101" s="2">
         <v>20</v>
@@ -5250,7 +5250,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="2">
-        <v>0.0008209999999999999</v>
+        <v>821</v>
       </c>
       <c r="D102" s="2">
         <v>20</v>
@@ -5294,7 +5294,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="2">
-        <v>0.0008259999999999999</v>
+        <v>826</v>
       </c>
       <c r="D103" s="2">
         <v>20</v>
@@ -5338,7 +5338,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="2">
-        <v>0.0008309999999999999</v>
+        <v>831</v>
       </c>
       <c r="D104" s="2">
         <v>20</v>
@@ -5382,7 +5382,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="2">
-        <v>0.0008359999999999999</v>
+        <v>836</v>
       </c>
       <c r="D105" s="2">
         <v>20</v>
@@ -5426,7 +5426,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="2">
-        <v>0.0008399999999999999</v>
+        <v>840</v>
       </c>
       <c r="D106" s="2">
         <v>20</v>
@@ -5470,7 +5470,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="2">
-        <v>0.0008449999999999999</v>
+        <v>845</v>
       </c>
       <c r="D107" s="2">
         <v>20</v>
@@ -5514,7 +5514,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="2">
-        <v>0.00085</v>
+        <v>850</v>
       </c>
       <c r="D108" s="2">
         <v>20</v>
@@ -5558,7 +5558,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="2">
-        <v>0.000855</v>
+        <v>855</v>
       </c>
       <c r="D109" s="2">
         <v>20</v>
@@ -5602,7 +5602,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="2">
-        <v>0.000861</v>
+        <v>861</v>
       </c>
       <c r="D110" s="2">
         <v>20</v>
@@ -5646,7 +5646,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="2">
-        <v>0.0008690000000000001</v>
+        <v>869.0000000000001</v>
       </c>
       <c r="D111" s="2">
         <v>20</v>
@@ -5690,7 +5690,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="2">
-        <v>0.0008759999999999999</v>
+        <v>875.9999999999999</v>
       </c>
       <c r="D112" s="2">
         <v>20</v>
@@ -5734,7 +5734,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="2">
-        <v>0.000884</v>
+        <v>884</v>
       </c>
       <c r="D113" s="2">
         <v>20</v>
@@ -5778,7 +5778,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="2">
-        <v>0.000892</v>
+        <v>892</v>
       </c>
       <c r="D114" s="2">
         <v>20</v>
@@ -5822,7 +5822,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="2">
-        <v>0.0009009999999999999</v>
+        <v>900.9999999999999</v>
       </c>
       <c r="D115" s="2">
         <v>20</v>
@@ -5866,7 +5866,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="2">
-        <v>0.0009109999999999999</v>
+        <v>910.9999999999999</v>
       </c>
       <c r="D116" s="2">
         <v>20</v>
@@ -5910,7 +5910,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="2">
-        <v>0.00092</v>
+        <v>920</v>
       </c>
       <c r="D117" s="2">
         <v>20</v>
@@ -5954,7 +5954,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="2">
-        <v>0.0009300000000000001</v>
+        <v>930</v>
       </c>
       <c r="D118" s="2">
         <v>20</v>
@@ -5998,7 +5998,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="2">
-        <v>0.0009390000000000001</v>
+        <v>939</v>
       </c>
       <c r="D119" s="2">
         <v>20</v>
@@ -6042,7 +6042,7 @@
         <v>118</v>
       </c>
       <c r="C120" s="2">
-        <v>0.0009479999999999999</v>
+        <v>948</v>
       </c>
       <c r="D120" s="2">
         <v>20</v>
@@ -6086,7 +6086,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="2">
-        <v>0.0009570000000000001</v>
+        <v>957.0000000000001</v>
       </c>
       <c r="D121" s="2">
         <v>20</v>
@@ -6130,7 +6130,7 @@
         <v>120</v>
       </c>
       <c r="C122" s="2">
-        <v>0.000966</v>
+        <v>966</v>
       </c>
       <c r="D122" s="2">
         <v>20</v>
@@ -6174,7 +6174,7 @@
         <v>121</v>
       </c>
       <c r="C123" s="2">
-        <v>0.000975</v>
+        <v>975</v>
       </c>
       <c r="D123" s="2">
         <v>20</v>
@@ -6218,7 +6218,7 @@
         <v>122</v>
       </c>
       <c r="C124" s="2">
-        <v>0.0009840000000000001</v>
+        <v>984.0000000000001</v>
       </c>
       <c r="D124" s="2">
         <v>20</v>
@@ -6262,7 +6262,7 @@
         <v>123</v>
       </c>
       <c r="C125" s="2">
-        <v>0.000993</v>
+        <v>993</v>
       </c>
       <c r="D125" s="2">
         <v>20</v>
@@ -6306,7 +6306,7 @@
         <v>124</v>
       </c>
       <c r="C126" s="2">
-        <v>0.001001</v>
+        <v>1001</v>
       </c>
       <c r="D126" s="2">
         <v>20</v>
@@ -6350,7 +6350,7 @@
         <v>125</v>
       </c>
       <c r="C127" s="2">
-        <v>0.00101</v>
+        <v>1010</v>
       </c>
       <c r="D127" s="2">
         <v>20</v>
@@ -6394,7 +6394,7 @@
         <v>126</v>
       </c>
       <c r="C128" s="2">
-        <v>0.001019</v>
+        <v>1019</v>
       </c>
       <c r="D128" s="2">
         <v>20</v>
@@ -6438,7 +6438,7 @@
         <v>127</v>
       </c>
       <c r="C129" s="2">
-        <v>0.001026</v>
+        <v>1026</v>
       </c>
       <c r="D129" s="2">
         <v>20</v>
@@ -6482,7 +6482,7 @@
         <v>128</v>
       </c>
       <c r="C130" s="2">
-        <v>0.001033</v>
+        <v>1033</v>
       </c>
       <c r="D130" s="2">
         <v>20</v>
@@ -6526,7 +6526,7 @@
         <v>129</v>
       </c>
       <c r="C131" s="2">
-        <v>0.001039</v>
+        <v>1039</v>
       </c>
       <c r="D131" s="2">
         <v>20</v>
@@ -6570,7 +6570,7 @@
         <v>130</v>
       </c>
       <c r="C132" s="2">
-        <v>0.001044</v>
+        <v>1044</v>
       </c>
       <c r="D132" s="2">
         <v>20</v>
@@ -6614,7 +6614,7 @@
         <v>131</v>
       </c>
       <c r="C133" s="2">
-        <v>0.001049</v>
+        <v>1049</v>
       </c>
       <c r="D133" s="2">
         <v>20</v>
@@ -6658,7 +6658,7 @@
         <v>132</v>
       </c>
       <c r="C134" s="2">
-        <v>0.001052</v>
+        <v>1052</v>
       </c>
       <c r="D134" s="2">
         <v>20</v>
@@ -6702,7 +6702,7 @@
         <v>133</v>
       </c>
       <c r="C135" s="2">
-        <v>0.001056</v>
+        <v>1056</v>
       </c>
       <c r="D135" s="2">
         <v>20</v>
@@ -6746,7 +6746,7 @@
         <v>134</v>
       </c>
       <c r="C136" s="2">
-        <v>0.001059</v>
+        <v>1059</v>
       </c>
       <c r="D136" s="2">
         <v>20</v>
@@ -6790,7 +6790,7 @@
         <v>135</v>
       </c>
       <c r="C137" s="2">
-        <v>0.001062</v>
+        <v>1062</v>
       </c>
       <c r="D137" s="2">
         <v>20</v>
@@ -6834,7 +6834,7 @@
         <v>136</v>
       </c>
       <c r="C138" s="2">
-        <v>0.001065</v>
+        <v>1065</v>
       </c>
       <c r="D138" s="2">
         <v>20</v>
@@ -6878,7 +6878,7 @@
         <v>137</v>
       </c>
       <c r="C139" s="2">
-        <v>0.001067</v>
+        <v>1067</v>
       </c>
       <c r="D139" s="2">
         <v>20</v>
@@ -6922,7 +6922,7 @@
         <v>138</v>
       </c>
       <c r="C140" s="2">
-        <v>0.001071</v>
+        <v>1071</v>
       </c>
       <c r="D140" s="2">
         <v>20</v>
@@ -6966,7 +6966,7 @@
         <v>139</v>
       </c>
       <c r="C141" s="2">
-        <v>0.001075</v>
+        <v>1075</v>
       </c>
       <c r="D141" s="2">
         <v>20</v>
@@ -7010,7 +7010,7 @@
         <v>140</v>
       </c>
       <c r="C142" s="2">
-        <v>0.00108</v>
+        <v>1080</v>
       </c>
       <c r="D142" s="2">
         <v>20</v>
@@ -7054,7 +7054,7 @@
         <v>141</v>
       </c>
       <c r="C143" s="2">
-        <v>0.001085</v>
+        <v>1085</v>
       </c>
       <c r="D143" s="2">
         <v>20</v>
@@ -7098,7 +7098,7 @@
         <v>142</v>
       </c>
       <c r="C144" s="2">
-        <v>0.00109</v>
+        <v>1090</v>
       </c>
       <c r="D144" s="2">
         <v>20</v>
@@ -7142,7 +7142,7 @@
         <v>143</v>
       </c>
       <c r="C145" s="2">
-        <v>0.001096</v>
+        <v>1096</v>
       </c>
       <c r="D145" s="2">
         <v>20</v>
@@ -7186,7 +7186,7 @@
         <v>144</v>
       </c>
       <c r="C146" s="2">
-        <v>0.001101</v>
+        <v>1101</v>
       </c>
       <c r="D146" s="2">
         <v>20</v>
@@ -7230,7 +7230,7 @@
         <v>145</v>
       </c>
       <c r="C147" s="2">
-        <v>0.001107</v>
+        <v>1107</v>
       </c>
       <c r="D147" s="2">
         <v>20</v>
@@ -7274,7 +7274,7 @@
         <v>146</v>
       </c>
       <c r="C148" s="2">
-        <v>0.001114</v>
+        <v>1114</v>
       </c>
       <c r="D148" s="2">
         <v>20</v>
@@ -7318,7 +7318,7 @@
         <v>147</v>
       </c>
       <c r="C149" s="2">
-        <v>0.001121</v>
+        <v>1121</v>
       </c>
       <c r="D149" s="2">
         <v>20</v>
@@ -7362,7 +7362,7 @@
         <v>148</v>
       </c>
       <c r="C150" s="2">
-        <v>0.001128</v>
+        <v>1128</v>
       </c>
       <c r="D150" s="2">
         <v>20</v>
@@ -7406,7 +7406,7 @@
         <v>149</v>
       </c>
       <c r="C151" s="2">
-        <v>0.001137</v>
+        <v>1137</v>
       </c>
       <c r="D151" s="2">
         <v>20</v>
@@ -7450,7 +7450,7 @@
         <v>150</v>
       </c>
       <c r="C152" s="2">
-        <v>0.001145</v>
+        <v>1145</v>
       </c>
       <c r="D152" s="2">
         <v>20</v>
@@ -7494,7 +7494,7 @@
         <v>151</v>
       </c>
       <c r="C153" s="2">
-        <v>0.001152</v>
+        <v>1152</v>
       </c>
       <c r="D153" s="2">
         <v>20</v>
@@ -7538,7 +7538,7 @@
         <v>152</v>
       </c>
       <c r="C154" s="2">
-        <v>0.001159</v>
+        <v>1159</v>
       </c>
       <c r="D154" s="2">
         <v>20</v>
@@ -7582,7 +7582,7 @@
         <v>153</v>
       </c>
       <c r="C155" s="2">
-        <v>0.001165</v>
+        <v>1165</v>
       </c>
       <c r="D155" s="2">
         <v>20</v>
@@ -7626,7 +7626,7 @@
         <v>154</v>
       </c>
       <c r="C156" s="2">
-        <v>0.001171</v>
+        <v>1171</v>
       </c>
       <c r="D156" s="2">
         <v>20</v>
@@ -7670,7 +7670,7 @@
         <v>155</v>
       </c>
       <c r="C157" s="2">
-        <v>0.001176</v>
+        <v>1176</v>
       </c>
       <c r="D157" s="2">
         <v>20</v>
@@ -7714,7 +7714,7 @@
         <v>156</v>
       </c>
       <c r="C158" s="2">
-        <v>0.001179</v>
+        <v>1179</v>
       </c>
       <c r="D158" s="2">
         <v>20</v>
@@ -7758,7 +7758,7 @@
         <v>157</v>
       </c>
       <c r="C159" s="2">
-        <v>0.001181</v>
+        <v>1181</v>
       </c>
       <c r="D159" s="2">
         <v>20</v>
@@ -7802,7 +7802,7 @@
         <v>158</v>
       </c>
       <c r="C160" s="2">
-        <v>0.001184</v>
+        <v>1184</v>
       </c>
       <c r="D160" s="2">
         <v>20</v>
@@ -7846,7 +7846,7 @@
         <v>159</v>
       </c>
       <c r="C161" s="2">
-        <v>0.001187</v>
+        <v>1187</v>
       </c>
       <c r="D161" s="2">
         <v>20</v>
@@ -7890,7 +7890,7 @@
         <v>160</v>
       </c>
       <c r="C162" s="2">
-        <v>0.001189</v>
+        <v>1189</v>
       </c>
       <c r="D162" s="2">
         <v>20</v>
@@ -7934,7 +7934,7 @@
         <v>161</v>
       </c>
       <c r="C163" s="2">
-        <v>0.001191</v>
+        <v>1191</v>
       </c>
       <c r="D163" s="2">
         <v>20</v>
@@ -7978,7 +7978,7 @@
         <v>162</v>
       </c>
       <c r="C164" s="2">
-        <v>0.001194</v>
+        <v>1194</v>
       </c>
       <c r="D164" s="2">
         <v>20</v>
@@ -8022,7 +8022,7 @@
         <v>163</v>
       </c>
       <c r="C165" s="2">
-        <v>0.001195</v>
+        <v>1195</v>
       </c>
       <c r="D165" s="2">
         <v>20</v>
@@ -8066,7 +8066,7 @@
         <v>164</v>
       </c>
       <c r="C166" s="2">
-        <v>0.001196</v>
+        <v>1196</v>
       </c>
       <c r="D166" s="2">
         <v>20</v>
@@ -8110,7 +8110,7 @@
         <v>165</v>
       </c>
       <c r="C167" s="2">
-        <v>0.001198</v>
+        <v>1198</v>
       </c>
       <c r="D167" s="2">
         <v>20</v>
@@ -8154,7 +8154,7 @@
         <v>166</v>
       </c>
       <c r="C168" s="2">
-        <v>0.001201</v>
+        <v>1201</v>
       </c>
       <c r="D168" s="2">
         <v>20</v>
@@ -8198,7 +8198,7 @@
         <v>167</v>
       </c>
       <c r="C169" s="2">
-        <v>0.001204</v>
+        <v>1204</v>
       </c>
       <c r="D169" s="2">
         <v>20</v>
@@ -8242,7 +8242,7 @@
         <v>168</v>
       </c>
       <c r="C170" s="2">
-        <v>0.001207</v>
+        <v>1207</v>
       </c>
       <c r="D170" s="2">
         <v>20</v>
@@ -8286,7 +8286,7 @@
         <v>169</v>
       </c>
       <c r="C171" s="2">
-        <v>0.00121</v>
+        <v>1210</v>
       </c>
       <c r="D171" s="2">
         <v>20</v>
@@ -8330,7 +8330,7 @@
         <v>170</v>
       </c>
       <c r="C172" s="2">
-        <v>0.001214</v>
+        <v>1214</v>
       </c>
       <c r="D172" s="2">
         <v>20</v>
@@ -8374,7 +8374,7 @@
         <v>171</v>
       </c>
       <c r="C173" s="2">
-        <v>0.001218</v>
+        <v>1218</v>
       </c>
       <c r="D173" s="2">
         <v>20</v>
@@ -8418,7 +8418,7 @@
         <v>172</v>
       </c>
       <c r="C174" s="2">
-        <v>0.001222</v>
+        <v>1222</v>
       </c>
       <c r="D174" s="2">
         <v>20</v>
@@ -8462,7 +8462,7 @@
         <v>173</v>
       </c>
       <c r="C175" s="2">
-        <v>0.001227</v>
+        <v>1227</v>
       </c>
       <c r="D175" s="2">
         <v>20</v>
@@ -8506,7 +8506,7 @@
         <v>174</v>
       </c>
       <c r="C176" s="2">
-        <v>0.001232</v>
+        <v>1232</v>
       </c>
       <c r="D176" s="2">
         <v>20</v>
@@ -8550,7 +8550,7 @@
         <v>175</v>
       </c>
       <c r="C177" s="2">
-        <v>0.001239</v>
+        <v>1239</v>
       </c>
       <c r="D177" s="2">
         <v>20</v>
@@ -8594,7 +8594,7 @@
         <v>176</v>
       </c>
       <c r="C178" s="2">
-        <v>0.001244</v>
+        <v>1244</v>
       </c>
       <c r="D178" s="2">
         <v>20</v>
@@ -8638,7 +8638,7 @@
         <v>177</v>
       </c>
       <c r="C179" s="2">
-        <v>0.001249</v>
+        <v>1249</v>
       </c>
       <c r="D179" s="2">
         <v>20</v>
@@ -8682,7 +8682,7 @@
         <v>178</v>
       </c>
       <c r="C180" s="2">
-        <v>0.001254</v>
+        <v>1254</v>
       </c>
       <c r="D180" s="2">
         <v>20</v>
@@ -8726,7 +8726,7 @@
         <v>179</v>
       </c>
       <c r="C181" s="2">
-        <v>0.001258</v>
+        <v>1258</v>
       </c>
       <c r="D181" s="2">
         <v>20</v>
@@ -8770,7 +8770,7 @@
         <v>180</v>
       </c>
       <c r="C182" s="2">
-        <v>0.001263</v>
+        <v>1263</v>
       </c>
       <c r="D182" s="2">
         <v>20</v>
@@ -8814,7 +8814,7 @@
         <v>181</v>
       </c>
       <c r="C183" s="2">
-        <v>0.001268</v>
+        <v>1268</v>
       </c>
       <c r="D183" s="2">
         <v>20</v>
@@ -8858,7 +8858,7 @@
         <v>182</v>
       </c>
       <c r="C184" s="2">
-        <v>0.001273</v>
+        <v>1273</v>
       </c>
       <c r="D184" s="2">
         <v>20</v>
@@ -8902,7 +8902,7 @@
         <v>183</v>
       </c>
       <c r="C185" s="2">
-        <v>0.001279</v>
+        <v>1279</v>
       </c>
       <c r="D185" s="2">
         <v>20</v>
@@ -8946,7 +8946,7 @@
         <v>184</v>
       </c>
       <c r="C186" s="2">
-        <v>0.001286</v>
+        <v>1286</v>
       </c>
       <c r="D186" s="2">
         <v>20</v>
@@ -8990,7 +8990,7 @@
         <v>185</v>
       </c>
       <c r="C187" s="2">
-        <v>0.001293</v>
+        <v>1293</v>
       </c>
       <c r="D187" s="2">
         <v>20</v>
@@ -9034,7 +9034,7 @@
         <v>186</v>
       </c>
       <c r="C188" s="2">
-        <v>0.0013</v>
+        <v>1300</v>
       </c>
       <c r="D188" s="2">
         <v>20</v>
@@ -9078,7 +9078,7 @@
         <v>187</v>
       </c>
       <c r="C189" s="2">
-        <v>0.001308</v>
+        <v>1308</v>
       </c>
       <c r="D189" s="2">
         <v>20</v>
@@ -9122,7 +9122,7 @@
         <v>188</v>
       </c>
       <c r="C190" s="2">
-        <v>0.001315</v>
+        <v>1315</v>
       </c>
       <c r="D190" s="2">
         <v>20</v>
@@ -9166,7 +9166,7 @@
         <v>189</v>
       </c>
       <c r="C191" s="2">
-        <v>0.001322</v>
+        <v>1322</v>
       </c>
       <c r="D191" s="2">
         <v>20</v>
@@ -9210,7 +9210,7 @@
         <v>190</v>
       </c>
       <c r="C192" s="2">
-        <v>0.00133</v>
+        <v>1330</v>
       </c>
       <c r="D192" s="2">
         <v>20</v>
@@ -9254,7 +9254,7 @@
         <v>191</v>
       </c>
       <c r="C193" s="2">
-        <v>0.001338</v>
+        <v>1338</v>
       </c>
       <c r="D193" s="2">
         <v>20</v>
@@ -9298,7 +9298,7 @@
         <v>192</v>
       </c>
       <c r="C194" s="2">
-        <v>0.001346</v>
+        <v>1346</v>
       </c>
       <c r="D194" s="2">
         <v>20</v>
@@ -9342,7 +9342,7 @@
         <v>193</v>
       </c>
       <c r="C195" s="2">
-        <v>0.001353</v>
+        <v>1353</v>
       </c>
       <c r="D195" s="2">
         <v>20</v>
@@ -9386,7 +9386,7 @@
         <v>194</v>
       </c>
       <c r="C196" s="2">
-        <v>0.00136</v>
+        <v>1360</v>
       </c>
       <c r="D196" s="2">
         <v>20</v>
@@ -9430,7 +9430,7 @@
         <v>195</v>
       </c>
       <c r="C197" s="2">
-        <v>0.001368</v>
+        <v>1368</v>
       </c>
       <c r="D197" s="2">
         <v>20</v>
@@ -9474,7 +9474,7 @@
         <v>196</v>
       </c>
       <c r="C198" s="2">
-        <v>0.001375</v>
+        <v>1375</v>
       </c>
       <c r="D198" s="2">
         <v>20</v>
@@ -9518,7 +9518,7 @@
         <v>197</v>
       </c>
       <c r="C199" s="2">
-        <v>0.001382</v>
+        <v>1382</v>
       </c>
       <c r="D199" s="2">
         <v>20</v>
@@ -9562,7 +9562,7 @@
         <v>198</v>
       </c>
       <c r="C200" s="2">
-        <v>0.001389</v>
+        <v>1389</v>
       </c>
       <c r="D200" s="2">
         <v>20</v>
@@ -9606,7 +9606,7 @@
         <v>199</v>
       </c>
       <c r="C201" s="2">
-        <v>0.001395</v>
+        <v>1395</v>
       </c>
       <c r="D201" s="2">
         <v>20</v>
@@ -9650,7 +9650,7 @@
         <v>200</v>
       </c>
       <c r="C202" s="2">
-        <v>0.001401</v>
+        <v>1401</v>
       </c>
       <c r="D202" s="2">
         <v>20</v>
@@ -9694,7 +9694,7 @@
         <v>201</v>
       </c>
       <c r="C203" s="2">
-        <v>0.001406</v>
+        <v>1406</v>
       </c>
       <c r="D203" s="2">
         <v>20</v>
@@ -9738,7 +9738,7 @@
         <v>202</v>
       </c>
       <c r="C204" s="2">
-        <v>0.001409</v>
+        <v>1409</v>
       </c>
       <c r="D204" s="2">
         <v>20</v>
@@ -9782,7 +9782,7 @@
         <v>203</v>
       </c>
       <c r="C205" s="2">
-        <v>0.001412</v>
+        <v>1412</v>
       </c>
       <c r="D205" s="2">
         <v>20</v>
@@ -9826,7 +9826,7 @@
         <v>204</v>
       </c>
       <c r="C206" s="2">
-        <v>0.001414</v>
+        <v>1414</v>
       </c>
       <c r="D206" s="2">
         <v>20</v>
@@ -9870,7 +9870,7 @@
         <v>205</v>
       </c>
       <c r="C207" s="2">
-        <v>0.001415</v>
+        <v>1415</v>
       </c>
       <c r="D207" s="2">
         <v>20</v>
@@ -9914,7 +9914,7 @@
         <v>206</v>
       </c>
       <c r="C208" s="2">
-        <v>0.001418</v>
+        <v>1418</v>
       </c>
       <c r="D208" s="2">
         <v>20</v>
@@ -9958,7 +9958,7 @@
         <v>207</v>
       </c>
       <c r="C209" s="2">
-        <v>0.001422</v>
+        <v>1422</v>
       </c>
       <c r="D209" s="2">
         <v>20</v>
@@ -10002,7 +10002,7 @@
         <v>208</v>
       </c>
       <c r="C210" s="2">
-        <v>0.001426</v>
+        <v>1426</v>
       </c>
       <c r="D210" s="2">
         <v>20</v>
@@ -10046,7 +10046,7 @@
         <v>209</v>
       </c>
       <c r="C211" s="2">
-        <v>0.001431</v>
+        <v>1431</v>
       </c>
       <c r="D211" s="2">
         <v>20</v>
@@ -10090,7 +10090,7 @@
         <v>210</v>
       </c>
       <c r="C212" s="2">
-        <v>0.001434</v>
+        <v>1434</v>
       </c>
       <c r="D212" s="2">
         <v>20</v>
@@ -10134,7 +10134,7 @@
         <v>211</v>
       </c>
       <c r="C213" s="2">
-        <v>0.001438</v>
+        <v>1438</v>
       </c>
       <c r="D213" s="2">
         <v>20</v>
@@ -10178,7 +10178,7 @@
         <v>212</v>
       </c>
       <c r="C214" s="2">
-        <v>0.00144</v>
+        <v>1440</v>
       </c>
       <c r="D214" s="2">
         <v>20</v>
@@ -10222,7 +10222,7 @@
         <v>213</v>
       </c>
       <c r="C215" s="2">
-        <v>0.001442</v>
+        <v>1442</v>
       </c>
       <c r="D215" s="2">
         <v>20</v>
@@ -10266,7 +10266,7 @@
         <v>214</v>
       </c>
       <c r="C216" s="2">
-        <v>0.001445</v>
+        <v>1445</v>
       </c>
       <c r="D216" s="2">
         <v>20</v>
@@ -10310,7 +10310,7 @@
         <v>215</v>
       </c>
       <c r="C217" s="2">
-        <v>0.001447</v>
+        <v>1447</v>
       </c>
       <c r="D217" s="2">
         <v>20</v>
@@ -10354,7 +10354,7 @@
         <v>216</v>
       </c>
       <c r="C218" s="2">
-        <v>0.001449</v>
+        <v>1449</v>
       </c>
       <c r="D218" s="2">
         <v>20</v>
@@ -10398,7 +10398,7 @@
         <v>217</v>
       </c>
       <c r="C219" s="2">
-        <v>0.001451</v>
+        <v>1451</v>
       </c>
       <c r="D219" s="2">
         <v>20</v>
@@ -10442,7 +10442,7 @@
         <v>218</v>
       </c>
       <c r="C220" s="2">
-        <v>0.001454</v>
+        <v>1454</v>
       </c>
       <c r="D220" s="2">
         <v>20</v>
@@ -10486,7 +10486,7 @@
         <v>219</v>
       </c>
       <c r="C221" s="2">
-        <v>0.001458</v>
+        <v>1458</v>
       </c>
       <c r="D221" s="2">
         <v>20</v>
@@ -10530,7 +10530,7 @@
         <v>220</v>
       </c>
       <c r="C222" s="2">
-        <v>0.001464</v>
+        <v>1464</v>
       </c>
       <c r="D222" s="2">
         <v>20</v>
@@ -10574,7 +10574,7 @@
         <v>221</v>
       </c>
       <c r="C223" s="2">
-        <v>0.001469</v>
+        <v>1469</v>
       </c>
       <c r="D223" s="2">
         <v>20</v>
@@ -10618,7 +10618,7 @@
         <v>222</v>
       </c>
       <c r="C224" s="2">
-        <v>0.001473</v>
+        <v>1473</v>
       </c>
       <c r="D224" s="2">
         <v>20</v>
@@ -10662,7 +10662,7 @@
         <v>223</v>
       </c>
       <c r="C225" s="2">
-        <v>0.001479</v>
+        <v>1479</v>
       </c>
       <c r="D225" s="2">
         <v>20</v>
@@ -10706,7 +10706,7 @@
         <v>224</v>
       </c>
       <c r="C226" s="2">
-        <v>0.001486</v>
+        <v>1486</v>
       </c>
       <c r="D226" s="2">
         <v>20</v>
@@ -10750,7 +10750,7 @@
         <v>225</v>
       </c>
       <c r="C227" s="2">
-        <v>0.001495</v>
+        <v>1495</v>
       </c>
       <c r="D227" s="2">
         <v>20</v>
@@ -10794,7 +10794,7 @@
         <v>226</v>
       </c>
       <c r="C228" s="2">
-        <v>0.001502</v>
+        <v>1502</v>
       </c>
       <c r="D228" s="2">
         <v>20</v>
@@ -10838,7 +10838,7 @@
         <v>227</v>
       </c>
       <c r="C229" s="2">
-        <v>0.001511</v>
+        <v>1511</v>
       </c>
       <c r="D229" s="2">
         <v>20</v>
@@ -10882,7 +10882,7 @@
         <v>228</v>
       </c>
       <c r="C230" s="2">
-        <v>0.001518</v>
+        <v>1518</v>
       </c>
       <c r="D230" s="2">
         <v>20</v>
@@ -10926,7 +10926,7 @@
         <v>229</v>
       </c>
       <c r="C231" s="2">
-        <v>0.001524</v>
+        <v>1524</v>
       </c>
       <c r="D231" s="2">
         <v>20</v>
@@ -10970,7 +10970,7 @@
         <v>230</v>
       </c>
       <c r="C232" s="2">
-        <v>0.001529</v>
+        <v>1529</v>
       </c>
       <c r="D232" s="2">
         <v>20</v>
@@ -11014,7 +11014,7 @@
         <v>231</v>
       </c>
       <c r="C233" s="2">
-        <v>0.001534</v>
+        <v>1534</v>
       </c>
       <c r="D233" s="2">
         <v>20</v>
@@ -11058,7 +11058,7 @@
         <v>232</v>
       </c>
       <c r="C234" s="2">
-        <v>0.001538</v>
+        <v>1538</v>
       </c>
       <c r="D234" s="2">
         <v>20</v>
@@ -11102,7 +11102,7 @@
         <v>233</v>
       </c>
       <c r="C235" s="2">
-        <v>0.001542</v>
+        <v>1542</v>
       </c>
       <c r="D235" s="2">
         <v>20</v>
@@ -11146,7 +11146,7 @@
         <v>234</v>
       </c>
       <c r="C236" s="2">
-        <v>0.001548</v>
+        <v>1548</v>
       </c>
       <c r="D236" s="2">
         <v>20</v>
@@ -11190,7 +11190,7 @@
         <v>235</v>
       </c>
       <c r="C237" s="2">
-        <v>0.001551</v>
+        <v>1551</v>
       </c>
       <c r="D237" s="2">
         <v>20</v>
@@ -11234,7 +11234,7 @@
         <v>236</v>
       </c>
       <c r="C238" s="2">
-        <v>0.001559</v>
+        <v>1559</v>
       </c>
       <c r="D238" s="2">
         <v>20</v>
@@ -11278,7 +11278,7 @@
         <v>237</v>
       </c>
       <c r="C239" s="2">
-        <v>0.001563</v>
+        <v>1563</v>
       </c>
       <c r="D239" s="2">
         <v>20</v>
@@ -11322,7 +11322,7 @@
         <v>238</v>
       </c>
       <c r="C240" s="2">
-        <v>0.001568</v>
+        <v>1568</v>
       </c>
       <c r="D240" s="2">
         <v>20</v>
@@ -11366,7 +11366,7 @@
         <v>239</v>
       </c>
       <c r="C241" s="2">
-        <v>0.001573</v>
+        <v>1573</v>
       </c>
       <c r="D241" s="2">
         <v>20</v>
@@ -11410,7 +11410,7 @@
         <v>240</v>
       </c>
       <c r="C242" s="2">
-        <v>0.001579</v>
+        <v>1579</v>
       </c>
       <c r="D242" s="2">
         <v>20</v>
@@ -11454,7 +11454,7 @@
         <v>241</v>
       </c>
       <c r="C243" s="2">
-        <v>0.001584</v>
+        <v>1584</v>
       </c>
       <c r="D243" s="2">
         <v>20</v>
@@ -11498,7 +11498,7 @@
         <v>242</v>
       </c>
       <c r="C244" s="2">
-        <v>0.00159</v>
+        <v>1590</v>
       </c>
       <c r="D244" s="2">
         <v>20</v>
@@ -11542,7 +11542,7 @@
         <v>243</v>
       </c>
       <c r="C245" s="2">
-        <v>0.001595</v>
+        <v>1595</v>
       </c>
       <c r="D245" s="2">
         <v>20</v>
@@ -11586,7 +11586,7 @@
         <v>244</v>
       </c>
       <c r="C246" s="2">
-        <v>0.001601</v>
+        <v>1601</v>
       </c>
       <c r="D246" s="2">
         <v>20</v>
@@ -11630,7 +11630,7 @@
         <v>245</v>
       </c>
       <c r="C247" s="2">
-        <v>0.001607</v>
+        <v>1607</v>
       </c>
       <c r="D247" s="2">
         <v>20</v>
@@ -11674,7 +11674,7 @@
         <v>246</v>
       </c>
       <c r="C248" s="2">
-        <v>0.001613</v>
+        <v>1613</v>
       </c>
       <c r="D248" s="2">
         <v>20</v>
@@ -11718,7 +11718,7 @@
         <v>247</v>
       </c>
       <c r="C249" s="2">
-        <v>0.001619</v>
+        <v>1619</v>
       </c>
       <c r="D249" s="2">
         <v>20</v>
@@ -11762,7 +11762,7 @@
         <v>248</v>
       </c>
       <c r="C250" s="2">
-        <v>0.001625</v>
+        <v>1625</v>
       </c>
       <c r="D250" s="2">
         <v>20</v>
@@ -11806,7 +11806,7 @@
         <v>249</v>
       </c>
       <c r="C251" s="2">
-        <v>0.001631</v>
+        <v>1631</v>
       </c>
       <c r="D251" s="2">
         <v>20</v>
@@ -11850,7 +11850,7 @@
         <v>250</v>
       </c>
       <c r="C252" s="2">
-        <v>0.001637</v>
+        <v>1637</v>
       </c>
       <c r="D252" s="2">
         <v>20</v>
@@ -11894,7 +11894,7 @@
         <v>251</v>
       </c>
       <c r="C253" s="2">
-        <v>0.001643</v>
+        <v>1643</v>
       </c>
       <c r="D253" s="2">
         <v>20</v>
@@ -11938,7 +11938,7 @@
         <v>252</v>
       </c>
       <c r="C254" s="2">
-        <v>0.001648</v>
+        <v>1648</v>
       </c>
       <c r="D254" s="2">
         <v>20</v>
@@ -11982,7 +11982,7 @@
         <v>253</v>
       </c>
       <c r="C255" s="2">
-        <v>0.001654</v>
+        <v>1654</v>
       </c>
       <c r="D255" s="2">
         <v>20</v>
@@ -12026,7 +12026,7 @@
         <v>254</v>
       </c>
       <c r="C256" s="2">
-        <v>0.00166</v>
+        <v>1660</v>
       </c>
       <c r="D256" s="2">
         <v>20</v>
@@ -12070,7 +12070,7 @@
         <v>255</v>
       </c>
       <c r="C257" s="2">
-        <v>0.001666</v>
+        <v>1666</v>
       </c>
       <c r="D257" s="2">
         <v>20</v>
@@ -12114,7 +12114,7 @@
         <v>256</v>
       </c>
       <c r="C258" s="2">
-        <v>0.001671</v>
+        <v>1671</v>
       </c>
       <c r="D258" s="2">
         <v>20</v>
@@ -12158,7 +12158,7 @@
         <v>257</v>
       </c>
       <c r="C259" s="2">
-        <v>0.001676</v>
+        <v>1676</v>
       </c>
       <c r="D259" s="2">
         <v>20</v>
@@ -12202,7 +12202,7 @@
         <v>258</v>
       </c>
       <c r="C260" s="2">
-        <v>0.00168</v>
+        <v>1680</v>
       </c>
       <c r="D260" s="2">
         <v>20</v>
@@ -12246,7 +12246,7 @@
         <v>259</v>
       </c>
       <c r="C261" s="2">
-        <v>0.001685</v>
+        <v>1685</v>
       </c>
       <c r="D261" s="2">
         <v>20</v>
@@ -12290,7 +12290,7 @@
         <v>260</v>
       </c>
       <c r="C262" s="2">
-        <v>0.00169</v>
+        <v>1690</v>
       </c>
       <c r="D262" s="2">
         <v>20</v>
@@ -12334,7 +12334,7 @@
         <v>261</v>
       </c>
       <c r="C263" s="2">
-        <v>0.001695</v>
+        <v>1695</v>
       </c>
       <c r="D263" s="2">
         <v>20</v>
@@ -12378,7 +12378,7 @@
         <v>262</v>
       </c>
       <c r="C264" s="2">
-        <v>0.0017</v>
+        <v>1700</v>
       </c>
       <c r="D264" s="2">
         <v>20</v>
@@ -12422,7 +12422,7 @@
         <v>263</v>
       </c>
       <c r="C265" s="2">
-        <v>0.001704</v>
+        <v>1704</v>
       </c>
       <c r="D265" s="2">
         <v>20</v>
@@ -12466,7 +12466,7 @@
         <v>264</v>
       </c>
       <c r="C266" s="2">
-        <v>0.001709</v>
+        <v>1709</v>
       </c>
       <c r="D266" s="2">
         <v>20</v>
@@ -12510,7 +12510,7 @@
         <v>265</v>
       </c>
       <c r="C267" s="2">
-        <v>0.001713</v>
+        <v>1713</v>
       </c>
       <c r="D267" s="2">
         <v>20</v>
@@ -12554,7 +12554,7 @@
         <v>266</v>
       </c>
       <c r="C268" s="2">
-        <v>0.001718</v>
+        <v>1718</v>
       </c>
       <c r="D268" s="2">
         <v>20</v>
@@ -12598,7 +12598,7 @@
         <v>267</v>
       </c>
       <c r="C269" s="2">
-        <v>0.001723</v>
+        <v>1723</v>
       </c>
       <c r="D269" s="2">
         <v>20</v>
@@ -12642,7 +12642,7 @@
         <v>268</v>
       </c>
       <c r="C270" s="2">
-        <v>0.001729</v>
+        <v>1729</v>
       </c>
       <c r="D270" s="2">
         <v>20</v>
@@ -12686,7 +12686,7 @@
         <v>269</v>
       </c>
       <c r="C271" s="2">
-        <v>0.001735</v>
+        <v>1735</v>
       </c>
       <c r="D271" s="2">
         <v>20</v>
@@ -12730,7 +12730,7 @@
         <v>270</v>
       </c>
       <c r="C272" s="2">
-        <v>0.001742</v>
+        <v>1742</v>
       </c>
       <c r="D272" s="2">
         <v>20</v>
@@ -12774,7 +12774,7 @@
         <v>271</v>
       </c>
       <c r="C273" s="2">
-        <v>0.001748</v>
+        <v>1748</v>
       </c>
       <c r="D273" s="2">
         <v>20</v>
@@ -12818,7 +12818,7 @@
         <v>272</v>
       </c>
       <c r="C274" s="2">
-        <v>0.001755</v>
+        <v>1755</v>
       </c>
       <c r="D274" s="2">
         <v>20</v>
@@ -12862,7 +12862,7 @@
         <v>273</v>
       </c>
       <c r="C275" s="2">
-        <v>0.001761</v>
+        <v>1761</v>
       </c>
       <c r="D275" s="2">
         <v>20</v>
@@ -12906,7 +12906,7 @@
         <v>274</v>
       </c>
       <c r="C276" s="2">
-        <v>0.001767</v>
+        <v>1767</v>
       </c>
       <c r="D276" s="2">
         <v>20</v>
@@ -12950,7 +12950,7 @@
         <v>275</v>
       </c>
       <c r="C277" s="2">
-        <v>0.001774</v>
+        <v>1774</v>
       </c>
       <c r="D277" s="2">
         <v>20</v>
@@ -12994,7 +12994,7 @@
         <v>276</v>
       </c>
       <c r="C278" s="2">
-        <v>0.00178</v>
+        <v>1780</v>
       </c>
       <c r="D278" s="2">
         <v>20</v>
@@ -13038,7 +13038,7 @@
         <v>277</v>
       </c>
       <c r="C279" s="2">
-        <v>0.001786</v>
+        <v>1786</v>
       </c>
       <c r="D279" s="2">
         <v>20</v>
@@ -13082,7 +13082,7 @@
         <v>278</v>
       </c>
       <c r="C280" s="2">
-        <v>0.001791</v>
+        <v>1791</v>
       </c>
       <c r="D280" s="2">
         <v>20</v>
@@ -13126,7 +13126,7 @@
         <v>279</v>
       </c>
       <c r="C281" s="2">
-        <v>0.001796</v>
+        <v>1796</v>
       </c>
       <c r="D281" s="2">
         <v>20</v>
@@ -13170,7 +13170,7 @@
         <v>280</v>
       </c>
       <c r="C282" s="2">
-        <v>0.001802</v>
+        <v>1802</v>
       </c>
       <c r="D282" s="2">
         <v>20</v>
@@ -13214,7 +13214,7 @@
         <v>281</v>
       </c>
       <c r="C283" s="2">
-        <v>0.001807</v>
+        <v>1807</v>
       </c>
       <c r="D283" s="2">
         <v>20</v>
@@ -13258,7 +13258,7 @@
         <v>282</v>
       </c>
       <c r="C284" s="2">
-        <v>0.001813</v>
+        <v>1813</v>
       </c>
       <c r="D284" s="2">
         <v>20</v>
@@ -13302,7 +13302,7 @@
         <v>283</v>
       </c>
       <c r="C285" s="2">
-        <v>0.001819</v>
+        <v>1819</v>
       </c>
       <c r="D285" s="2">
         <v>20</v>
@@ -13346,7 +13346,7 @@
         <v>284</v>
       </c>
       <c r="C286" s="2">
-        <v>0.001825</v>
+        <v>1825</v>
       </c>
       <c r="D286" s="2">
         <v>20</v>
@@ -13390,7 +13390,7 @@
         <v>285</v>
       </c>
       <c r="C287" s="2">
-        <v>0.001831</v>
+        <v>1831</v>
       </c>
       <c r="D287" s="2">
         <v>20</v>
@@ -13434,7 +13434,7 @@
         <v>286</v>
       </c>
       <c r="C288" s="2">
-        <v>0.001838</v>
+        <v>1838</v>
       </c>
       <c r="D288" s="2">
         <v>20</v>
@@ -13478,7 +13478,7 @@
         <v>287</v>
       </c>
       <c r="C289" s="2">
-        <v>0.001844</v>
+        <v>1844</v>
       </c>
       <c r="D289" s="2">
         <v>20</v>
@@ -13522,7 +13522,7 @@
         <v>288</v>
       </c>
       <c r="C290" s="2">
-        <v>0.00185</v>
+        <v>1850</v>
       </c>
       <c r="D290" s="2">
         <v>20</v>
@@ -13566,7 +13566,7 @@
         <v>289</v>
       </c>
       <c r="C291" s="2">
-        <v>0.001856</v>
+        <v>1856</v>
       </c>
       <c r="D291" s="2">
         <v>20</v>
@@ -13610,7 +13610,7 @@
         <v>290</v>
       </c>
       <c r="C292" s="2">
-        <v>0.001862</v>
+        <v>1862</v>
       </c>
       <c r="D292" s="2">
         <v>20</v>
@@ -13654,7 +13654,7 @@
         <v>291</v>
       </c>
       <c r="C293" s="2">
-        <v>0.001868</v>
+        <v>1868</v>
       </c>
       <c r="D293" s="2">
         <v>20</v>
@@ -13698,7 +13698,7 @@
         <v>292</v>
       </c>
       <c r="C294" s="2">
-        <v>0.001874</v>
+        <v>1874</v>
       </c>
       <c r="D294" s="2">
         <v>20</v>
@@ -13742,7 +13742,7 @@
         <v>293</v>
       </c>
       <c r="C295" s="2">
-        <v>0.00188</v>
+        <v>1880</v>
       </c>
       <c r="D295" s="2">
         <v>20</v>
@@ -13786,7 +13786,7 @@
         <v>294</v>
       </c>
       <c r="C296" s="2">
-        <v>0.001886</v>
+        <v>1886</v>
       </c>
       <c r="D296" s="2">
         <v>20</v>
@@ -13830,7 +13830,7 @@
         <v>295</v>
       </c>
       <c r="C297" s="2">
-        <v>0.001892</v>
+        <v>1892</v>
       </c>
       <c r="D297" s="2">
         <v>20</v>
@@ -13874,7 +13874,7 @@
         <v>296</v>
       </c>
       <c r="C298" s="2">
-        <v>0.001898</v>
+        <v>1898</v>
       </c>
       <c r="D298" s="2">
         <v>20</v>
@@ -13918,7 +13918,7 @@
         <v>297</v>
       </c>
       <c r="C299" s="2">
-        <v>0.001903</v>
+        <v>1903</v>
       </c>
       <c r="D299" s="2">
         <v>20</v>
@@ -13962,7 +13962,7 @@
         <v>298</v>
       </c>
       <c r="C300" s="2">
-        <v>0.001909</v>
+        <v>1909</v>
       </c>
       <c r="D300" s="2">
         <v>20</v>
@@ -14006,7 +14006,7 @@
         <v>299</v>
       </c>
       <c r="C301" s="2">
-        <v>0.001914</v>
+        <v>1914</v>
       </c>
       <c r="D301" s="2">
         <v>20</v>
@@ -14050,7 +14050,7 @@
         <v>300</v>
       </c>
       <c r="C302" s="2">
-        <v>0.00192</v>
+        <v>1920</v>
       </c>
       <c r="D302" s="2">
         <v>20</v>
@@ -14094,7 +14094,7 @@
         <v>301</v>
       </c>
       <c r="C303" s="2">
-        <v>0.001925</v>
+        <v>1925</v>
       </c>
       <c r="D303" s="2">
         <v>20</v>
@@ -14138,7 +14138,7 @@
         <v>302</v>
       </c>
       <c r="C304" s="2">
-        <v>0.001931</v>
+        <v>1931</v>
       </c>
       <c r="D304" s="2">
         <v>20</v>
@@ -14182,7 +14182,7 @@
         <v>303</v>
       </c>
       <c r="C305" s="2">
-        <v>0.001937</v>
+        <v>1937</v>
       </c>
       <c r="D305" s="2">
         <v>20</v>
@@ -14226,7 +14226,7 @@
         <v>304</v>
       </c>
       <c r="C306" s="2">
-        <v>0.001942</v>
+        <v>1942</v>
       </c>
       <c r="D306" s="2">
         <v>20</v>
@@ -14270,7 +14270,7 @@
         <v>305</v>
       </c>
       <c r="C307" s="2">
-        <v>0.001947</v>
+        <v>1947</v>
       </c>
       <c r="D307" s="2">
         <v>20</v>
@@ -14314,7 +14314,7 @@
         <v>306</v>
       </c>
       <c r="C308" s="2">
-        <v>0.001951</v>
+        <v>1951</v>
       </c>
       <c r="D308" s="2">
         <v>20</v>
@@ -14358,7 +14358,7 @@
         <v>307</v>
       </c>
       <c r="C309" s="2">
-        <v>0.001954</v>
+        <v>1954</v>
       </c>
       <c r="D309" s="2">
         <v>20</v>
@@ -14402,7 +14402,7 @@
         <v>308</v>
       </c>
       <c r="C310" s="2">
-        <v>0.001958</v>
+        <v>1958</v>
       </c>
       <c r="D310" s="2">
         <v>20</v>
@@ -14446,7 +14446,7 @@
         <v>309</v>
       </c>
       <c r="C311" s="2">
-        <v>0.001962</v>
+        <v>1962</v>
       </c>
       <c r="D311" s="2">
         <v>20</v>
@@ -14490,7 +14490,7 @@
         <v>310</v>
       </c>
       <c r="C312" s="2">
-        <v>0.001965</v>
+        <v>1965</v>
       </c>
       <c r="D312" s="2">
         <v>20</v>
@@ -14534,7 +14534,7 @@
         <v>311</v>
       </c>
       <c r="C313" s="2">
-        <v>0.00197</v>
+        <v>1970</v>
       </c>
       <c r="D313" s="2">
         <v>20</v>
@@ -14578,7 +14578,7 @@
         <v>312</v>
       </c>
       <c r="C314" s="2">
-        <v>0.001976</v>
+        <v>1976</v>
       </c>
       <c r="D314" s="2">
         <v>20</v>
@@ -14622,7 +14622,7 @@
         <v>313</v>
       </c>
       <c r="C315" s="2">
-        <v>0.001981</v>
+        <v>1981</v>
       </c>
       <c r="D315" s="2">
         <v>20</v>
@@ -14666,7 +14666,7 @@
         <v>314</v>
       </c>
       <c r="C316" s="2">
-        <v>0.001987</v>
+        <v>1987</v>
       </c>
       <c r="D316" s="2">
         <v>20</v>
@@ -14710,7 +14710,7 @@
         <v>315</v>
       </c>
       <c r="C317" s="2">
-        <v>0.001992</v>
+        <v>1992</v>
       </c>
       <c r="D317" s="2">
         <v>20</v>
@@ -14754,7 +14754,7 @@
         <v>316</v>
       </c>
       <c r="C318" s="2">
-        <v>0.001997</v>
+        <v>1997</v>
       </c>
       <c r="D318" s="2">
         <v>20</v>
@@ -14798,7 +14798,7 @@
         <v>317</v>
       </c>
       <c r="C319" s="2">
-        <v>0.002003</v>
+        <v>2003</v>
       </c>
       <c r="D319" s="2">
         <v>20</v>
@@ -14842,7 +14842,7 @@
         <v>318</v>
       </c>
       <c r="C320" s="2">
-        <v>0.002011</v>
+        <v>2011</v>
       </c>
       <c r="D320" s="2">
         <v>20</v>
@@ -14886,7 +14886,7 @@
         <v>319</v>
       </c>
       <c r="C321" s="2">
-        <v>0.002016</v>
+        <v>2016</v>
       </c>
       <c r="D321" s="2">
         <v>20</v>
@@ -14930,7 +14930,7 @@
         <v>320</v>
       </c>
       <c r="C322" s="2">
-        <v>0.002022</v>
+        <v>2022</v>
       </c>
       <c r="D322" s="2">
         <v>20</v>
@@ -14974,7 +14974,7 @@
         <v>321</v>
       </c>
       <c r="C323" s="2">
-        <v>0.002028</v>
+        <v>2028</v>
       </c>
       <c r="D323" s="2">
         <v>20</v>
@@ -15018,7 +15018,7 @@
         <v>322</v>
       </c>
       <c r="C324" s="2">
-        <v>0.002034</v>
+        <v>2034</v>
       </c>
       <c r="D324" s="2">
         <v>20</v>
@@ -15062,7 +15062,7 @@
         <v>323</v>
       </c>
       <c r="C325" s="2">
-        <v>0.002041</v>
+        <v>2041</v>
       </c>
       <c r="D325" s="2">
         <v>20</v>
@@ -15106,7 +15106,7 @@
         <v>324</v>
       </c>
       <c r="C326" s="2">
-        <v>0.002046</v>
+        <v>2046</v>
       </c>
       <c r="D326" s="2">
         <v>20</v>
@@ -15150,7 +15150,7 @@
         <v>325</v>
       </c>
       <c r="C327" s="2">
-        <v>0.002051</v>
+        <v>2051</v>
       </c>
       <c r="D327" s="2">
         <v>20</v>
@@ -15194,7 +15194,7 @@
         <v>326</v>
       </c>
       <c r="C328" s="2">
-        <v>0.002056</v>
+        <v>2056</v>
       </c>
       <c r="D328" s="2">
         <v>20</v>
@@ -15238,7 +15238,7 @@
         <v>327</v>
       </c>
       <c r="C329" s="2">
-        <v>0.002059</v>
+        <v>2059</v>
       </c>
       <c r="D329" s="2">
         <v>20</v>
@@ -15282,7 +15282,7 @@
         <v>328</v>
       </c>
       <c r="C330" s="2">
-        <v>0.002063</v>
+        <v>2063</v>
       </c>
       <c r="D330" s="2">
         <v>20</v>
@@ -15326,7 +15326,7 @@
         <v>329</v>
       </c>
       <c r="C331" s="2">
-        <v>0.002065</v>
+        <v>2065</v>
       </c>
       <c r="D331" s="2">
         <v>20</v>

</xml_diff>